<commit_message>
Set valid AMPL model in Excel input files
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks106/09-experts16-tastks106.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks106/09-experts16-tastks106.xlsx
@@ -783,7 +783,7 @@
     <t xml:space="preserve">highs</t>
   </si>
   <si>
-    <t xml:space="preserve">ubday</t>
+    <t xml:space="preserve">solid-ubday</t>
   </si>
   <si>
     <t xml:space="preserve">For all charts</t>
@@ -1624,7 +1624,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>